<commit_message>
add a gtk2 symbols crush error's debug file and some else
</commit_message>
<xml_diff>
--- a/paper/paper.xlsx
+++ b/paper/paper.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="208">
   <si>
     <t>title</t>
   </si>
@@ -1478,6 +1478,12 @@
   </si>
   <si>
     <t>写的有点儿LOW。。。</t>
+  </si>
+  <si>
+    <t>Semantic Mapping for Mobile Robots in Indoor Scenes A Survey</t>
+  </si>
+  <si>
+    <t>Xiaoning Han  , Shuailong Li  , Xiaohui Wang and Weijia Zhou</t>
   </si>
 </sst>
 </file>
@@ -1486,8 +1492,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
@@ -1551,16 +1557,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1575,19 +1587,20 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -1595,9 +1608,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1611,29 +1639,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -1641,15 +1656,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -1665,15 +1672,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1694,7 +1700,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1706,7 +1712,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1718,7 +1730,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1736,7 +1772,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1748,103 +1868,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1856,25 +1880,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1888,22 +1894,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1923,17 +1924,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1962,6 +1959,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1980,8 +1986,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1993,10 +1999,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2005,16 +2011,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2026,112 +2032,112 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2508,10 +2514,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" outlineLevelCol="6"/>
@@ -3447,6 +3453,17 @@
       </c>
       <c r="F49" s="1" t="s">
         <v>205</v>
+      </c>
+    </row>
+    <row r="50" ht="62.4" spans="1:3">
+      <c r="A50" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C50" s="1">
+        <v>2021</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add a paper Translation file
</commit_message>
<xml_diff>
--- a/paper/paper.xlsx
+++ b/paper/paper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9420" tabRatio="227"/>
+    <workbookView windowWidth="28800" windowHeight="13548" tabRatio="227"/>
   </bookViews>
   <sheets>
     <sheet name="slam" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="214">
   <si>
     <t>title</t>
   </si>
@@ -1484,6 +1484,25 @@
   </si>
   <si>
     <t>Xiaoning Han  , Shuailong Li  , Xiaohui Wang and Weijia Zhou</t>
+  </si>
+  <si>
+    <t>室内场景下实时地三维语义地图构建</t>
+  </si>
+  <si>
+    <t>单吉超，李秀智</t>
+  </si>
+  <si>
+    <t>仪器仪表学报</t>
+  </si>
+  <si>
+    <t>基于深度残差网络( DＲN) 的像素级图像语义分割和三维同时定位与建图( SLAM) 相融合的三维语义地图构建方法。首先，采用一种联合中值滤波算法进行深度图像的修复，使用改进的迭代最近点( ICP) 算法得到相机估计
+位姿以及基于随机蕨类的闭环检测构建出三维环境地图; 其次，采用优化的深度残差网络对输入的图像实现较精准的像素语义级别的预测与分割; 最后，采用贝叶斯更新方法，渐进式的将图像分割获取的语义分类标签迁移到重建的室内三维模型中，获得完整的三维语义地图。实验表明，所设计的方法可以在实际的、复杂环境下实时地构建语义地图。</t>
+  </si>
+  <si>
+    <t>实时的移动机器人语义地图构建系统</t>
+  </si>
+  <si>
+    <t>李秀智，李尚宇</t>
   </si>
 </sst>
 </file>
@@ -1491,10 +1510,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -1557,6 +1576,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -1571,40 +1628,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1613,14 +1641,6 @@
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1655,17 +1675,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1700,6 +1719,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1712,7 +1755,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1724,13 +1839,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1742,73 +1857,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1832,43 +1887,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1891,71 +1910,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1985,6 +1939,71 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -1999,10 +2018,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2011,16 +2030,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2032,13 +2051,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2053,91 +2072,91 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2514,9 +2533,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
       <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
@@ -3464,6 +3483,37 @@
       </c>
       <c r="C50" s="1">
         <v>2021</v>
+      </c>
+    </row>
+    <row r="51" ht="124.8" spans="1:5">
+      <c r="A51" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C51" s="1">
+        <v>2019</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C52" s="1">
+        <v>2017</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
move and fix files
</commit_message>
<xml_diff>
--- a/paper/paper.xlsx
+++ b/paper/paper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13548" tabRatio="227"/>
+    <workbookView windowWidth="23040" windowHeight="10308" tabRatio="227"/>
   </bookViews>
   <sheets>
     <sheet name="slam" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="218">
   <si>
     <t>title</t>
   </si>
@@ -1503,6 +1503,18 @@
   </si>
   <si>
     <t>李秀智，李尚宇</t>
+  </si>
+  <si>
+    <t>RDS-SLAM_Real-Time_Dynamic_SLAM_Using_Semantic_Segmentation_Methods.pdf</t>
+  </si>
+  <si>
+    <t>YUBAO LIU AND JUN MIURA</t>
+  </si>
+  <si>
+    <t>a real-time visual dynamic SLAM algorithm that is built on ORB-SLAM3 and adds a semantic thread and a semantic-based optimization thread for robust tracking and mapping in dynamic environments in real-time.相比于其他将CNN语义识别放到track线程中，此文提出并行语义识别线程，不损耗track时间。提出了一种尽可能获得最新语义信息算法，从而适用不同速度分割算法。使用移动概率更新和传播语义信息，该概率保存在地图中，并使用数据关联算法去除outliers</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 开源！https://github.com/yubaoliu/RDS-SLAM.git</t>
   </si>
 </sst>
 </file>
@@ -1511,9 +1523,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -1578,37 +1590,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1622,25 +1611,31 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1675,8 +1670,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1691,14 +1695,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1719,13 +1731,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1737,7 +1755,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1749,7 +1839,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1761,19 +1869,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1785,121 +1911,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1910,6 +1922,45 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1937,56 +1988,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2010,6 +2011,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -2018,10 +2030,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2030,16 +2042,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2051,112 +2063,112 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2533,10 +2545,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" outlineLevelCol="6"/>
@@ -3514,6 +3526,26 @@
       </c>
       <c r="D52" s="1" t="s">
         <v>210</v>
+      </c>
+    </row>
+    <row r="58" ht="109.2" spans="1:6">
+      <c r="A58" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C58" s="1">
+        <v>2021</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update slambook_note.md and add understand_quaternion_cn.pdf
</commit_message>
<xml_diff>
--- a/paper/paper.xlsx
+++ b/paper/paper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="10308" tabRatio="227"/>
+    <workbookView windowWidth="28128" windowHeight="13548" tabRatio="227"/>
   </bookViews>
   <sheets>
     <sheet name="slam" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="232">
   <si>
     <t>title</t>
   </si>
@@ -1541,6 +1541,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>使用</t>
     </r>
     <r>
@@ -1564,6 +1571,28 @@
       </rPr>
       <t>实现自然语言到地图路径规划和定位的对应</t>
     </r>
+  </si>
+  <si>
+    <t>Semantic_SLAM_Based_on_Object_Detection_and_Improved_Octomap</t>
+  </si>
+  <si>
+    <t>LIANG ZHANG
+, LEQI WEI
+, PEIYI SHEN</t>
+  </si>
+  <si>
+    <t>直接用YOLO检测对象，然后剔除属于先验动态对象目标范围内的特征点，从而实现动态环境下的正确数据关联</t>
+  </si>
+  <si>
+    <t>A_Mobile_Robot_Visual_SLAM_System_With_Enhanced_Semantics_Segmentation</t>
+  </si>
+  <si>
+    <t>FENG LI
+, WENFENG CHEN
+, WEIFENG XU</t>
+  </si>
+  <si>
+    <t>使用Segment进行语义分割，然后剔除人与椅子等对象内的特征点</t>
   </si>
 </sst>
 </file>
@@ -1572,9 +1601,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -1638,6 +1667,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -1645,7 +1688,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1659,15 +1702,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1681,18 +1723,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1730,7 +1780,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1738,28 +1788,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1788,7 +1817,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1800,19 +1889,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1824,85 +1919,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1920,13 +1943,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1938,7 +1955,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1956,19 +1991,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1997,17 +2026,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2023,6 +2046,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2045,6 +2083,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -2055,30 +2108,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -2087,10 +2116,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2099,16 +2128,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2120,112 +2149,112 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2602,10 +2631,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="D107" sqref="D107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" outlineLevelCol="6"/>
@@ -3637,6 +3666,34 @@
       </c>
       <c r="F65" s="1" t="s">
         <v>225</v>
+      </c>
+    </row>
+    <row r="107" ht="62.4" spans="1:4">
+      <c r="A107" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C107" s="1">
+        <v>2018</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="110" ht="46.8" spans="1:4">
+      <c r="A110" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C110" s="1">
+        <v>2020</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>